<commit_message>
minority_percent column added to syn exp results
</commit_message>
<xml_diff>
--- a/data/prepared_results.xlsx
+++ b/data/prepared_results.xlsx
@@ -505,7 +505,7 @@
   <dimension ref="A1:K73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L69" sqref="L69"/>
+      <selection activeCell="A8" sqref="A8:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -621,11 +621,11 @@
         <v>27</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J8" si="0">C3/C$2</f>
+        <f t="shared" ref="J3:J7" si="0">C3/C$2</f>
         <v>2.6340511634629289</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K8" si="1">E3/E$2</f>
+        <f t="shared" ref="K3:K7" si="1">E3/E$2</f>
         <v>1.4087810469699646</v>
       </c>
     </row>
@@ -843,11 +843,11 @@
         <v>28</v>
       </c>
       <c r="J9">
-        <f t="shared" ref="J9:J14" si="2">C9/C$8</f>
+        <f t="shared" ref="J9:J13" si="2">C9/C$8</f>
         <v>1.0069891228882204</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="K9:K14" si="3">E9/E$8</f>
+        <f t="shared" ref="K9:K13" si="3">E9/E$8</f>
         <v>0.9999825717477574</v>
       </c>
     </row>
@@ -1065,11 +1065,11 @@
         <v>29</v>
       </c>
       <c r="J15">
-        <f t="shared" ref="J15:J20" si="4">C15/C$14</f>
+        <f t="shared" ref="J15:J19" si="4">C15/C$14</f>
         <v>0.96097560975609753</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="K15:K20" si="5">E15/E$14</f>
+        <f t="shared" ref="K15:K19" si="5">E15/E$14</f>
         <v>1</v>
       </c>
     </row>
@@ -1287,11 +1287,11 @@
         <v>29</v>
       </c>
       <c r="J21">
-        <f t="shared" ref="J21:J26" si="6">C21/C$20</f>
+        <f t="shared" ref="J21:J25" si="6">C21/C$20</f>
         <v>1.0049504950495047</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="K21:K26" si="7">E21/E$20</f>
+        <f t="shared" ref="K21:K25" si="7">E21/E$20</f>
         <v>1.000751476113795</v>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
         <v>30</v>
       </c>
       <c r="J27">
-        <f t="shared" ref="J27:J32" si="8">C27/C$26</f>
+        <f t="shared" ref="J27:J31" si="8">C27/C$26</f>
         <v>1.0023934030571198</v>
       </c>
       <c r="K27">

</xml_diff>